<commit_message>
Close #85, Close #86, Close #85
</commit_message>
<xml_diff>
--- a/01.Documentation/01.Diseño/Compatibilidad Producciones.xlsx
+++ b/01.Documentation/01.Diseño/Compatibilidad Producciones.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Team Dropbox\JRODRIGUEZ\Repositorios\01.Rover\01.Documentation\01.Diseño\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{844DDB31-1BDF-4144-95EB-1EA3473BBD6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F9CCD3-4A86-40DC-9439-80A863A0F1AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HARDWARE" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
   <si>
     <t>Fecha</t>
   </si>
@@ -233,6 +233,16 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>Produccion 5</t>
+  </si>
+  <si>
+    <t>Universal</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * Res. Balastro
+R19,R20 = 20R</t>
   </si>
 </sst>
 </file>
@@ -453,7 +463,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -490,6 +500,18 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -508,17 +530,8 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2027,15 +2040,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>228599</xdr:colOff>
+      <xdr:colOff>234552</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>21771</xdr:rowOff>
+      <xdr:rowOff>21772</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>489857</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>16328</xdr:rowOff>
+      <xdr:colOff>495810</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>261938</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2050,8 +2063,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4125685" y="1088571"/>
-          <a:ext cx="261258" cy="261257"/>
+          <a:off x="3865958" y="2212522"/>
+          <a:ext cx="261258" cy="240166"/>
         </a:xfrm>
         <a:prstGeom prst="mathMultiply">
           <a:avLst/>
@@ -2088,13 +2101,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>185057</xdr:colOff>
+      <xdr:colOff>196963</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>5442</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>446315</xdr:colOff>
+      <xdr:colOff>458221</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>266699</xdr:rowOff>
     </xdr:to>
@@ -2111,7 +2124,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6242957" y="1072242"/>
+          <a:off x="6007213" y="2196192"/>
           <a:ext cx="261258" cy="261257"/>
         </a:xfrm>
         <a:prstGeom prst="mathMultiply">
@@ -2329,6 +2342,1131 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>228599</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>24383</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="257556" cy="233171"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="image4.jpeg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C60F4A04-2F33-4D91-AD86-E03763EBD6B3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8943974" y="1667446"/>
+          <a:ext cx="257556" cy="233171"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>228599</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>10667</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="257556" cy="233171"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="image6.jpeg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{724B4357-E85F-4B5A-865C-9F51C4E1E426}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8943974" y="2201417"/>
+          <a:ext cx="257556" cy="233171"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>228599</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>16764</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="257556" cy="233171"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="image7.jpeg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D5DD8E0-6221-40C1-B093-03A5A8FDC266}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8943974" y="1933670"/>
+          <a:ext cx="257556" cy="233171"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>245363</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>15239</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="257556" cy="233171"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="image15.jpeg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{314CBADB-E009-468F-883D-1969154583A4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8234457" y="1658302"/>
+          <a:ext cx="257556" cy="233171"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>245363</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>9144</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="257556" cy="233171"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="image16.jpeg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F4ACB84-31FA-48FC-8E25-4A317590066B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8234457" y="1926050"/>
+          <a:ext cx="257556" cy="233171"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>228599</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>10668</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="257555" cy="236219"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="36" name="image17.jpeg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35AD46F4-AAFC-48BB-AD16-AF77367579A3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8217693" y="2201418"/>
+          <a:ext cx="257555" cy="236219"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>250371</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>16328</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="257555" cy="233172"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="44" name="image2.jpeg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D20D4CF7-B996-476B-814E-971E85E1B4B5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7513184" y="1659391"/>
+          <a:ext cx="257555" cy="233172"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>255814</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>21771</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="257555" cy="233172"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="47" name="image2.jpeg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBF9D60F-9730-474D-AB0D-F7CF3D9CBD09}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7518627" y="2212521"/>
+          <a:ext cx="257555" cy="233172"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>261937</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>29765</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="257555" cy="233171"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="52" name="image19.jpeg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D816E0E-ACF1-4234-B74B-2F8E710D7BB5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="988218" y="2494359"/>
+          <a:ext cx="257555" cy="233171"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>217883</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>15478</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="257555" cy="233171"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="53" name="image19.jpeg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7220B365-3FCD-4EF0-A814-6671DAEA55D8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2396727" y="2480072"/>
+          <a:ext cx="257555" cy="233171"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>251221</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>30956</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="257555" cy="233171"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="54" name="image19.jpeg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9012347F-4AD6-4A12-8B08-EED3B0D7FA4A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3156346" y="2495550"/>
+          <a:ext cx="257555" cy="233171"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>236934</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>22621</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="257555" cy="233171"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="55" name="image19.jpeg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3543A16C-C532-4B04-91A8-D524A0FBA454}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3868340" y="2487215"/>
+          <a:ext cx="257555" cy="233171"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>216693</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="257555" cy="233171"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="56" name="image19.jpeg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF8208E5-AD08-483B-A6C6-259D59CFA9EA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5300662" y="2478881"/>
+          <a:ext cx="257555" cy="233171"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>267891</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>11906</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="257555" cy="233171"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="57" name="image19.jpeg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6A3707A-8917-435A-B5D2-0043EFBC97EA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9709547" y="2476500"/>
+          <a:ext cx="257555" cy="233171"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>223837</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="257555" cy="233171"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="58" name="image19.jpeg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECA3571B-8B1F-4983-A472-E0756255BB1C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10391775" y="2497931"/>
+          <a:ext cx="257555" cy="233171"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>239316</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>36908</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="257555" cy="233171"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="59" name="image19.jpeg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{079ADCA7-56A7-4120-8BD7-14B30DFEEAD1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11133535" y="2501502"/>
+          <a:ext cx="257555" cy="233171"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>230982</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>22621</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="257555" cy="233171"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="60" name="image19.jpeg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8380E5C-1CA7-49C6-AC39-1383E86E380C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8946357" y="2487215"/>
+          <a:ext cx="257555" cy="233171"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>222647</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>32146</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="257555" cy="233171"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="61" name="image19.jpeg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58499704-DF55-48FE-8345-219557C56992}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8211741" y="2496740"/>
+          <a:ext cx="257555" cy="233171"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>41671</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="257555" cy="233171"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="62" name="image19.jpeg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7B0034E-A8B8-4B6F-949E-3E7A6220B8E8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7500938" y="2506265"/>
+          <a:ext cx="257555" cy="233171"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>259557</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>33336</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="257555" cy="233171"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="63" name="image19.jpeg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{024A9559-4ABA-46B9-A3EE-0FC32F27180D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6796088" y="2497930"/>
+          <a:ext cx="257555" cy="233171"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>194072</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="257555" cy="233171"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="66" name="image19.jpeg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF3A06B2-2223-4248-965A-81EFA9BF255D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6004322" y="2474119"/>
+          <a:ext cx="257555" cy="233171"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>222645</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>26193</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="257555" cy="233171"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="68" name="image19.jpeg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5852CAA5-57C0-44B2-8D7F-EB561AC2025A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4580333" y="2490787"/>
+          <a:ext cx="257555" cy="233171"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>226216</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>29765</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="257555" cy="233171"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="69" name="image19.jpeg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FEE29C19-798B-44B9-A86C-74333089D003}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1678779" y="2494359"/>
+          <a:ext cx="257555" cy="233171"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>232172</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>23813</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="257556" cy="233171"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="71" name="image16.jpeg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24640D40-30F8-43EF-8525-C6B29380CCC3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7494985" y="1940719"/>
+          <a:ext cx="257556" cy="233171"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>232172</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>35719</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="257556" cy="233171"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="72" name="image16.jpeg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{225F3825-CB94-4E82-85C4-DC0DCB8E5B60}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9673828" y="1952625"/>
+          <a:ext cx="257556" cy="233171"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2622,58 +3760,63 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:M11"/>
+  <dimension ref="A2:P12"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1">
         <f ca="1">TODAY()</f>
-        <v>45495</v>
+        <v>45552</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
+    <row r="5" spans="1:16" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="14" t="s">
+      <c r="C5" s="19"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="15"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="14" t="s">
+      <c r="F5" s="19"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="15"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="14" t="s">
+      <c r="I5" s="19"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="L5" s="15"/>
-      <c r="M5" s="16"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="O5" s="19"/>
+      <c r="P5" s="20"/>
     </row>
-    <row r="6" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="13"/>
+    <row r="6" spans="1:16" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="17"/>
       <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
@@ -2710,8 +3853,17 @@
       <c r="M6" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="N6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="7" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -2727,8 +3879,11 @@
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
     </row>
-    <row r="8" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>14</v>
       </c>
@@ -2744,8 +3899,11 @@
       <c r="K8" s="8"/>
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
     </row>
-    <row r="9" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>15</v>
       </c>
@@ -2763,45 +3921,84 @@
         <v>18</v>
       </c>
       <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="P9" s="6"/>
     </row>
-    <row r="10" spans="1:13" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:16" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+    </row>
+    <row r="11" spans="1:16" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="2" t="s">
+      <c r="I11" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="K11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L10" s="2" t="s">
+      <c r="L11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="M10" s="10"/>
+      <c r="M11" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="P11" s="10"/>
     </row>
-    <row r="11" spans="1:13" ht="46.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:16" ht="46.5" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="N5:P5"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="E5:G5"/>
@@ -2818,8 +4015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5522CA65-D719-4940-AB96-9D69370E64C7}">
   <dimension ref="A2:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2829,55 +4026,55 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="20">
-        <v>1</v>
+      <c r="B2" s="14">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="21">
-        <v>45495</v>
+      <c r="B3" s="15">
+        <v>45547</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="21" x14ac:dyDescent="0.2">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
     </row>
     <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="12" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="117.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="19">
-        <v>124</v>
-      </c>
-      <c r="B7" s="19">
-        <v>312</v>
-      </c>
-      <c r="C7" s="19" t="s">
+      <c r="A7" s="13">
+        <v>125</v>
+      </c>
+      <c r="B7" s="13">
+        <v>313</v>
+      </c>
+      <c r="C7" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="19">
-        <v>204</v>
+      <c r="D7" s="13">
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>